<commit_message>
Sample code, guides added
</commit_message>
<xml_diff>
--- a/Practical8/autophagosome.xlsx
+++ b/Practical8/autophagosome.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jefft/Desktop/ZJE/IBI(local)/git_repository/IBI1_2018-19/Practical8/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA98F9D0-90D9-B340-B80F-E96C981B4BB4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="21820" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -352,12 +346,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -365,15 +359,8 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -419,23 +406,15 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -477,7 +456,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -509,27 +488,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -561,24 +522,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -754,17 +697,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
-  <cols>
-    <col min="2" max="2" width="21.83203125" customWidth="1"/>
-    <col min="3" max="3" width="32.33203125" customWidth="1"/>
-    <col min="4" max="4" width="30.33203125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
@@ -1376,7 +1314,6 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>